<commit_message>
generated new translate_codes file
</commit_message>
<xml_diff>
--- a/data_in/translate_STAGE.xlsx
+++ b/data_in/translate_STAGE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\winfs-proj\data\proj\havgem\Mo-PROJEKTKATALOG\Uppdrag\HaV\Datavärdskapet_oceanografi_och_marinbiologi\2022\Städning\Translate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\codes_shark\codes\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE693777-9A6E-4775-9CF1-7C2F00495CE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21F3DD3-D31F-4AD2-8234-95C9A4E3A270}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="3250" xr2:uid="{1A0B3E34-E74F-4EB7-997F-926D3A9788AA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="103">
   <si>
     <t>AD</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>ns</t>
+  </si>
+  <si>
+    <t>&lt;use_nerc_name&gt;</t>
   </si>
 </sst>
 </file>
@@ -763,7 +766,7 @@
   <dimension ref="A1:K107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1277,6 +1280,12 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>102</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>

</xml_diff>